<commit_message>
Made changes in TravelInsurance excel file
</commit_message>
<xml_diff>
--- a/testData/PolicyBazar_TravelInsuranceData.xlsx
+++ b/testData/PolicyBazar_TravelInsuranceData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2406657_cognizant_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{345D0A3C-CBAB-4AD8-A1F1-2E99AB5766FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C023815-631E-4A5B-9202-5F6EA574F5DB}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{345D0A3C-CBAB-4AD8-A1F1-2E99AB5766FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D68134C-601B-4E6A-A29F-C401F1CC1608}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CECB4F61-37E2-4A0F-9D13-CADE1DBB676D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +41,12 @@
     <t>Country</t>
   </si>
   <si>
+    <t xml:space="preserve">Start Date       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End Date</t>
+  </si>
+  <si>
     <t>Number Of Travellers</t>
   </si>
   <si>
@@ -53,24 +59,18 @@
     <t>Travel Duration</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Date       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> End Date</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
     <t>2025/July/21</t>
   </si>
   <si>
+    <t>2025/August/25</t>
+  </si>
+  <si>
     <t>30 Days</t>
   </si>
   <si>
-    <t>2025/August/25</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
@@ -98,14 +98,14 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>2026/January/4</t>
+    <t>2025/October/4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,10 +177,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,44 +499,44 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -548,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -560,10 +556,10 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -586,7 +582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -609,12 +605,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>

</xml_diff>